<commit_message>
Updated index regressions with controls to include SBAC test scores
</commit_message>
<xml_diff>
--- a/out/xls/factoranalysis/indexhorserace/compcasehorserace_newindex.xlsx
+++ b/out/xls/factoranalysis/indexhorserace/compcasehorserace_newindex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Dropbox\Davis\Research Projects\Ed Lab GSR\caschls\out\xls\factoranalysis\indexhorserace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0591D3FF-C078-4D45-A07B-4B052FC9966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6A5D03-867C-49C5-A40A-EF2C60315F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9570" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compcasehorserace" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>-0.628***</t>
   </si>
@@ -39,39 +39,6 @@
     <t>0.311**</t>
   </si>
   <si>
-    <t>0.307**</t>
-  </si>
-  <si>
-    <t>0.286*</t>
-  </si>
-  <si>
-    <t>0.261*</t>
-  </si>
-  <si>
-    <t>0.306**</t>
-  </si>
-  <si>
-    <t>0.288*</t>
-  </si>
-  <si>
-    <t>0.270*</t>
-  </si>
-  <si>
-    <t>0.271*</t>
-  </si>
-  <si>
-    <t>(-0.25)</t>
-  </si>
-  <si>
-    <t>(-0.27)</t>
-  </si>
-  <si>
-    <t>(-0.22)</t>
-  </si>
-  <si>
-    <t>(-0.23)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -141,18 +108,9 @@
     <t>Teacher and Staff Quality</t>
   </si>
   <si>
-    <t>Student Support</t>
-  </si>
-  <si>
-    <t>Student Motivation</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
-    <t>NOTE: Reregressions are run using standardized z scores for all variables. These are multivariate regressions with all 4 index variables as regressors.</t>
-  </si>
-  <si>
     <t>Multivariate Value-Added Regressions on All Category Index: Complete Case Analysis</t>
   </si>
   <si>
@@ -409,6 +367,12 @@
   </si>
   <si>
     <t>(-2.28)</t>
+  </si>
+  <si>
+    <t>Counseling Support</t>
+  </si>
+  <si>
+    <t>NOTE: Regressions are run using standardized z scores for all variables. These are multivariate regressions with all 3 index variables as regressors.</t>
   </si>
 </sst>
 </file>
@@ -916,7 +880,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -926,6 +890,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1283,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1297,15 +1264,15 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1324,137 +1291,137 @@
     <row r="4" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1475,93 +1442,93 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -1582,93 +1549,93 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -1689,93 +1656,93 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
-        <v>0.188</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>4</v>
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-1.0500000000000001E-2</v>
       </c>
       <c r="H15" s="1">
-        <v>-2.86E-2</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="I15" s="1">
-        <v>-3.1199999999999999E-2</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="J15" s="1">
-        <v>-2.5999999999999999E-2</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="K15" s="1">
-        <v>-2.6800000000000001E-2</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>6</v>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="L15" s="1">
+        <v>-0.105</v>
+      </c>
+      <c r="M15" s="1">
+        <v>-0.112</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
-        <v>-1.76</v>
+        <v>-0.22</v>
       </c>
       <c r="C16" s="1">
-        <v>-1.23</v>
+        <v>-2.02</v>
       </c>
       <c r="D16" s="1">
-        <v>-2.65</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="E16" s="1">
-        <v>-2.2999999999999998</v>
-      </c>
-      <c r="F16" s="1">
-        <v>-2.19</v>
-      </c>
-      <c r="G16" s="1">
-        <v>-2.17</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="1">
-        <v>-2.8</v>
-      </c>
-      <c r="M16" s="1">
-        <v>-2.5</v>
-      </c>
-      <c r="N16" s="1">
-        <v>-2.35</v>
-      </c>
-      <c r="O16" s="1">
-        <v>-2.36</v>
+        <v>-0.51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-1.75</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-1.74</v>
+      </c>
+      <c r="J16" s="1">
+        <v>-1.79</v>
+      </c>
+      <c r="K16" s="1">
+        <v>-1.86</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1796,177 +1763,70 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.5900000000000001E-2</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4.6100000000000002E-2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>4.3400000000000001E-2</v>
-      </c>
-      <c r="F18" s="1">
-        <v>-1.4E-2</v>
-      </c>
-      <c r="G18" s="1">
-        <v>-1.0500000000000001E-2</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="L18" s="1">
-        <v>-0.105</v>
-      </c>
-      <c r="M18" s="1">
-        <v>-0.112</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
-        <v>-0.22</v>
-      </c>
-      <c r="C19" s="1">
-        <v>-2.02</v>
-      </c>
-      <c r="D19" s="1">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="E19" s="1">
-        <v>-0.51</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="1">
-        <v>-1.75</v>
-      </c>
-      <c r="I19" s="1">
-        <v>-1.74</v>
-      </c>
-      <c r="J19" s="1">
-        <v>-1.79</v>
-      </c>
-      <c r="K19" s="1">
-        <v>-1.86</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>125</v>
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
+        <v>288</v>
+      </c>
+      <c r="C18" s="5">
+        <v>288</v>
+      </c>
+      <c r="D18" s="5">
+        <v>284</v>
+      </c>
+      <c r="E18" s="5">
+        <v>284</v>
+      </c>
+      <c r="F18" s="5">
+        <v>284</v>
+      </c>
+      <c r="G18" s="5">
+        <v>284</v>
+      </c>
+      <c r="H18" s="5">
+        <v>284</v>
+      </c>
+      <c r="I18" s="5">
+        <v>284</v>
+      </c>
+      <c r="J18" s="5">
+        <v>284</v>
+      </c>
+      <c r="K18" s="5">
+        <v>284</v>
+      </c>
+      <c r="L18" s="5">
+        <v>284</v>
+      </c>
+      <c r="M18" s="5">
+        <v>284</v>
+      </c>
+      <c r="N18" s="5">
+        <v>284</v>
+      </c>
+      <c r="O18" s="5">
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1">
-        <v>288</v>
-      </c>
-      <c r="C21" s="1">
-        <v>288</v>
-      </c>
-      <c r="D21" s="1">
-        <v>284</v>
-      </c>
-      <c r="E21" s="1">
-        <v>284</v>
-      </c>
-      <c r="F21" s="1">
-        <v>284</v>
-      </c>
-      <c r="G21" s="1">
-        <v>284</v>
-      </c>
-      <c r="H21" s="1">
-        <v>284</v>
-      </c>
-      <c r="I21" s="1">
-        <v>284</v>
-      </c>
-      <c r="J21" s="1">
-        <v>284</v>
-      </c>
-      <c r="K21" s="1">
-        <v>284</v>
-      </c>
-      <c r="L21" s="1">
-        <v>284</v>
-      </c>
-      <c r="M21" s="1">
-        <v>284</v>
-      </c>
-      <c r="N21" s="1">
-        <v>284</v>
-      </c>
-      <c r="O21" s="1">
-        <v>284</v>
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>